<commit_message>
Update notebook "Global-fit Ishikawa's Ne beta parameters.ipynb" Add notebook "Reduce Ishikawa's coeffs.ipynb” Update data beta_neon_ishikawa.yaml Update table "parameters_He_Ne (reformatted).xlsx"
</commit_message>
<xml_diff>
--- a/Data/parameters_He_Ne (reformatted).xlsx
+++ b/Data/parameters_He_Ne (reformatted).xlsx
@@ -8,14 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daehyun/Documents/FERMI 20144077 Ueda/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D83C630-F32F-D24A-8CC5-CC86B6F011D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727CF0BF-7094-0843-9F58-D8D9992BAC9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45100" yWindow="460" windowWidth="25560" windowHeight="19480" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="42500" yWindow="480" windowWidth="25560" windowHeight="19480" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="He.0.0.9 w2w" sheetId="9" r:id="rId1"/>
     <sheet name="Ne.1.0.8 w2w" sheetId="10" r:id="rId2"/>
     <sheet name="Ne.0.0.5 wonly" sheetId="11" r:id="rId3"/>
+    <sheet name="good1_ne" sheetId="12" r:id="rId4"/>
+    <sheet name="good2_ne" sheetId="13" r:id="rId5"/>
+    <sheet name="good3_ne" sheetId="14" r:id="rId6"/>
+    <sheet name="good4_ne" sheetId="15" r:id="rId7"/>
+    <sheet name="k" sheetId="16" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="23">
   <si>
     <t>beta1</t>
   </si>
@@ -67,14 +72,48 @@
   <si>
     <t>beta1m3</t>
   </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>p_amp</t>
+  </si>
+  <si>
+    <t>p_arg</t>
+  </si>
+  <si>
+    <t>sp_amp</t>
+  </si>
+  <si>
+    <t>dp_amp</t>
+  </si>
+  <si>
+    <t>fdp_amp</t>
+  </si>
+  <si>
+    <t>sp_arg</t>
+  </si>
+  <si>
+    <t>dp_arg</t>
+  </si>
+  <si>
+    <t>fdp_arg</t>
+  </si>
+  <si>
+    <t>psp_amp</t>
+  </si>
+  <si>
+    <t>pdp_amp</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -112,7 +151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -148,11 +187,645 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="79">
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0000"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -308,20 +981,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E1581C30-C069-6C41-BABA-1C429C369E0E}" name="Table1" displayName="Table1" ref="A1:H33" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E1581C30-C069-6C41-BABA-1C429C369E0E}" name="Table1" displayName="Table1" ref="A1:H33" totalsRowShown="0" headerRowDxfId="78" dataDxfId="77">
   <autoFilter ref="A1:H33" xr:uid="{5A2F4E3C-6216-8A44-B44C-DC41925F48CF}"/>
   <sortState ref="A2:H33">
     <sortCondition ref="A1:A33"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{EBB224F5-2851-A244-A5AD-EEB7479118A2}" name="dataset" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{98D32EC9-E0E4-7A4D-B030-1A15ED90F7EB}" name="photon (eV)" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{5FEB3B01-1E66-3640-8D98-DF6243493A25}" name="phi (deg)" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{12877EDA-C127-6A44-A914-7B61346E1B4A}" name="beta1" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{41FF9D2F-DBF3-CB4A-A9A7-6E1F02E6FEDC}" name="beta2" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{09478A6E-A782-3342-A160-09612E259736}" name="beta3" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{F4EF1465-E339-5140-9DF2-3348F0148ED4}" name="beta4" dataDxfId="19"/>
-    <tableColumn id="9" xr3:uid="{83EC2B29-3C15-2040-9B91-46576B1EFBD5}" name="beta1m3" dataDxfId="18">
+    <tableColumn id="1" xr3:uid="{EBB224F5-2851-A244-A5AD-EEB7479118A2}" name="dataset" dataDxfId="76"/>
+    <tableColumn id="2" xr3:uid="{98D32EC9-E0E4-7A4D-B030-1A15ED90F7EB}" name="photon (eV)" dataDxfId="75"/>
+    <tableColumn id="3" xr3:uid="{5FEB3B01-1E66-3640-8D98-DF6243493A25}" name="phi (deg)" dataDxfId="74"/>
+    <tableColumn id="4" xr3:uid="{12877EDA-C127-6A44-A914-7B61346E1B4A}" name="beta1" dataDxfId="73"/>
+    <tableColumn id="5" xr3:uid="{41FF9D2F-DBF3-CB4A-A9A7-6E1F02E6FEDC}" name="beta2" dataDxfId="72"/>
+    <tableColumn id="6" xr3:uid="{09478A6E-A782-3342-A160-09612E259736}" name="beta3" dataDxfId="71"/>
+    <tableColumn id="7" xr3:uid="{F4EF1465-E339-5140-9DF2-3348F0148ED4}" name="beta4" dataDxfId="70"/>
+    <tableColumn id="9" xr3:uid="{83EC2B29-3C15-2040-9B91-46576B1EFBD5}" name="beta1m3" dataDxfId="69">
       <calculatedColumnFormula>Table1[[#This Row],[beta1]]-2/3*Table1[[#This Row],[beta3]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -330,20 +1003,20 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{49F98CB5-2CCA-914E-99AC-01EF4E0630CB}" name="Table13" displayName="Table13" ref="A1:H33" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{49F98CB5-2CCA-914E-99AC-01EF4E0630CB}" name="Table13" displayName="Table13" ref="A1:H33" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67">
   <autoFilter ref="A1:H33" xr:uid="{5426A37B-AC88-574B-8345-856314EF6161}"/>
   <sortState ref="A2:H33">
     <sortCondition ref="A1:A33"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{49790D79-1FF6-D341-B361-C121D15FCE21}" name="dataset" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{053C0271-54EC-5446-ADE7-CDB91FA9CBF9}" name="photon (eV)" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{1045FA6E-AB4F-5041-A2A6-676D2A80FBAA}" name="phi (deg)" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{A71DA1D1-EE48-FB42-9E10-CFF5CB2359F8}" name="beta1" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{2DB4ADCA-6CF3-F248-810E-6082C1100295}" name="beta2" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{8B709B2D-BFE0-4442-A171-2149EEFF1B45}" name="beta3" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{A0C26D95-2F39-C146-A4B3-BCFF54658EC9}" name="beta4" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{C87F7B48-ED25-3D48-93E4-BC0687725265}" name="beta1m3" dataDxfId="8">
+    <tableColumn id="1" xr3:uid="{49790D79-1FF6-D341-B361-C121D15FCE21}" name="dataset" dataDxfId="66"/>
+    <tableColumn id="2" xr3:uid="{053C0271-54EC-5446-ADE7-CDB91FA9CBF9}" name="photon (eV)" dataDxfId="65"/>
+    <tableColumn id="3" xr3:uid="{1045FA6E-AB4F-5041-A2A6-676D2A80FBAA}" name="phi (deg)" dataDxfId="64"/>
+    <tableColumn id="4" xr3:uid="{A71DA1D1-EE48-FB42-9E10-CFF5CB2359F8}" name="beta1" dataDxfId="63"/>
+    <tableColumn id="5" xr3:uid="{2DB4ADCA-6CF3-F248-810E-6082C1100295}" name="beta2" dataDxfId="62"/>
+    <tableColumn id="6" xr3:uid="{8B709B2D-BFE0-4442-A171-2149EEFF1B45}" name="beta3" dataDxfId="61"/>
+    <tableColumn id="7" xr3:uid="{A0C26D95-2F39-C146-A4B3-BCFF54658EC9}" name="beta4" dataDxfId="60"/>
+    <tableColumn id="10" xr3:uid="{C87F7B48-ED25-3D48-93E4-BC0687725265}" name="beta1m3" dataDxfId="59">
       <calculatedColumnFormula>Table13[[#This Row],[beta1]]-3/2*Table13[[#This Row],[beta3]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -352,20 +1025,113 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F05A4894-8C70-D642-85C3-3AB7CFBB4F28}" name="Table135" displayName="Table135" ref="A1:F5" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F05A4894-8C70-D642-85C3-3AB7CFBB4F28}" name="Table135" displayName="Table135" ref="A1:F5" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
   <autoFilter ref="A1:F5" xr:uid="{53E4CFBE-4728-384F-AC3E-37B66AF4A439}"/>
   <sortState ref="A2:F5">
     <sortCondition ref="A1:A5"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{13AA3944-170F-3846-AA70-1C1962C64192}" name="dataset" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{BD60D2D9-15A2-F545-AAFF-748850E64446}" name="photon (eV)" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{28273152-69FC-A241-BCA6-31BCEA8C2BEC}" name="beta1" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{33E9B38C-ACC9-0A49-9295-DACDF599E7FB}" name="beta2" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{407B9B6B-64D4-014F-A379-342916257ADC}" name="beta3" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{8826E549-F298-AB41-856D-6CC97B08EAB8}" name="beta4" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{13AA3944-170F-3846-AA70-1C1962C64192}" name="dataset" dataDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{BD60D2D9-15A2-F545-AAFF-748850E64446}" name="photon (eV)" dataDxfId="55"/>
+    <tableColumn id="4" xr3:uid="{28273152-69FC-A241-BCA6-31BCEA8C2BEC}" name="beta1" dataDxfId="54"/>
+    <tableColumn id="5" xr3:uid="{33E9B38C-ACC9-0A49-9295-DACDF599E7FB}" name="beta2" dataDxfId="53"/>
+    <tableColumn id="6" xr3:uid="{407B9B6B-64D4-014F-A379-342916257ADC}" name="beta3" dataDxfId="52"/>
+    <tableColumn id="7" xr3:uid="{8826E549-F298-AB41-856D-6CC97B08EAB8}" name="beta4" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{59DFE585-94CE-324E-80C4-17D5A8535F3A}" name="Table3" displayName="Table3" ref="A1:I4" totalsRowShown="0" headerRowDxfId="50">
+  <autoFilter ref="A1:I4" xr:uid="{8B5C4BC6-D08A-F342-B69E-95E18573CBD5}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{5BA34F36-7497-CA4F-999F-15736C5C90B3}" name="m" dataDxfId="49"/>
+    <tableColumn id="2" xr3:uid="{A0426779-3323-8542-8FAD-30E204B20D55}" name="sp_amp" dataDxfId="48"/>
+    <tableColumn id="3" xr3:uid="{684B6570-B9E4-704D-8176-FCA5A03A637E}" name="p_amp" dataDxfId="47"/>
+    <tableColumn id="4" xr3:uid="{ADC74BA0-1CC4-1C48-A1F6-685EBC267637}" name="dp_amp" dataDxfId="46"/>
+    <tableColumn id="5" xr3:uid="{2845C546-B0B7-214A-9B3A-94C4A1525E23}" name="fdp_amp" dataDxfId="45"/>
+    <tableColumn id="6" xr3:uid="{1E48FDEC-EE5F-7C46-A4AB-BA8213F216B3}" name="sp_arg" dataDxfId="44"/>
+    <tableColumn id="7" xr3:uid="{CD04CD5C-B6F2-9246-BDA1-EA343D3D5323}" name="p_arg" dataDxfId="43"/>
+    <tableColumn id="8" xr3:uid="{9B5BB2F1-9199-A844-952A-2F3D8A2919AF}" name="dp_arg" dataDxfId="42"/>
+    <tableColumn id="9" xr3:uid="{6B1CD9FD-B8D5-2043-9623-1AE12EBE013F}" name="fdp_arg" dataDxfId="41"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{AEAD797E-5610-6742-BF1C-D62A7ADBA7F0}" name="Table5" displayName="Table5" ref="A1:I4" totalsRowShown="0" headerRowDxfId="2" dataDxfId="40">
+  <autoFilter ref="A1:I4" xr:uid="{B4719746-BFD9-6D4E-8D94-4B12B338165F}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{647D98FB-251B-4542-BF7C-63F898E9AC7E}" name="m" dataDxfId="39"/>
+    <tableColumn id="2" xr3:uid="{2E22E77A-4173-0D4A-9A6F-7E47D1678087}" name="sp_amp" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{D6903029-EBD1-994F-97CC-EBA1ABF4E926}" name="p_amp" dataDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{3DF53176-C13B-7641-82D5-1BE402BDD02F}" name="dp_amp" dataDxfId="36"/>
+    <tableColumn id="5" xr3:uid="{1060BE76-3E32-1A48-9A41-0593EE6FE8C2}" name="fdp_amp" dataDxfId="35"/>
+    <tableColumn id="6" xr3:uid="{FFBFF49F-1059-1642-8A31-AD573823D3E3}" name="sp_arg" dataDxfId="34"/>
+    <tableColumn id="7" xr3:uid="{1D811937-AFDD-8D48-81C8-B33622C03534}" name="p_arg" dataDxfId="33"/>
+    <tableColumn id="8" xr3:uid="{E126B12C-EED2-324A-A8CC-51A76C96BAAD}" name="dp_arg" dataDxfId="32"/>
+    <tableColumn id="9" xr3:uid="{8C65ED6F-4B8F-3246-ABE2-AE3D22B29FF5}" name="fdp_arg" dataDxfId="31"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2A026460-1D43-9646-BB18-B4646ACDCF3D}" name="Table6" displayName="Table6" ref="A1:I4" totalsRowShown="0" headerRowDxfId="1" dataDxfId="30">
+  <autoFilter ref="A1:I4" xr:uid="{A8FC2363-68E6-1D4F-AF75-C41078FEDC29}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{67A1216D-8F66-8F47-9DDF-9779C464E009}" name="m" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{7A921D8C-3F15-E140-B838-5A1204B74685}" name="sp_amp" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{F8CDDF88-4BC2-1D4A-84BD-6353BF4B9E77}" name="p_amp" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{1481DC66-2D0E-E04E-B630-3C7741CE4CD0}" name="dp_amp" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{720417F9-6520-2C47-B50F-B0B73F912EED}" name="fdp_amp" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{826D4DF2-FA71-F24E-8ED5-A415C4A6D02B}" name="sp_arg" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{D5972777-E932-ED4A-8B82-9C8059F7E06E}" name="p_arg" dataDxfId="23"/>
+    <tableColumn id="8" xr3:uid="{8DE1440F-E3A9-014F-BD79-E3166B7C3A72}" name="dp_arg" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{19C76EA3-897A-3148-80AE-374F812A5850}" name="fdp_arg" dataDxfId="21"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{E38178F3-1826-3E4D-BBB2-2C0D6EDAE208}" name="Table7" displayName="Table7" ref="A1:I4" totalsRowShown="0" headerRowDxfId="0" dataDxfId="20">
+  <autoFilter ref="A1:I4" xr:uid="{DC15BAF1-E157-5A42-A33B-060096B22C67}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{FDE47AB7-D70F-3145-A921-E12C0BE05C94}" name="m" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{D43E9326-FEAF-EE49-A01C-CC943A2F4B91}" name="sp_amp" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{7BDC518E-90F1-4D47-A627-F285D44C0247}" name="p_amp" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{EC03AEAB-910C-CD4C-A25B-38E5F1590E5A}" name="dp_amp" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{608F44B2-D548-C349-A1C6-FE7BFEDBADE8}" name="fdp_amp" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{7E6BAB65-DA36-BC48-B2EB-1A3CFDB0CC8D}" name="sp_arg" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{45305CC1-A33F-8644-8440-E87A9BA944D8}" name="p_arg" dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{A4952650-FD28-5B48-8679-6D186F7D7ED6}" name="dp_arg" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{B0FF8D19-EC72-B44F-88D1-021AB69F405F}" name="fdp_arg" dataDxfId="11"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{763C1B8E-8E8C-1C43-AF64-24E938897D53}" name="Table19" displayName="Table19" ref="A1:F4" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:F4" xr:uid="{B629EAAC-C030-3144-A5C8-EA87A0850D51}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{678C78C9-26BE-E640-8E8C-8BD4C90EA1D8}" name="m" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{F4BE6F06-FE79-854C-A751-08C0116B4DA2}" name="sp_amp" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{5D349974-DB77-004C-A546-3F935BF8CE78}" name="psp_amp" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{914971F8-D9D5-3042-9BBD-39AA14A4A973}" name="pdp_amp" dataDxfId="5">
+      <calculatedColumnFormula>-SQRT(15)/10</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{1E5B610A-F2B0-C845-8B12-F74BAEE6BEAC}" name="dp_amp" dataDxfId="4">
+      <calculatedColumnFormula>SQRT(2)/2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{9597E78F-47B1-1F45-BC2F-077AD7E519D2}" name="fdp_amp" dataDxfId="3">
+      <calculatedColumnFormula>2*SQRT(15)/15</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -634,8 +1400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{299A2AA5-3F91-3F46-9BEF-D7AF19513A24}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2581,4 +3347,655 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F07D9F88-15BB-7E44-A02C-3321FE5E3C69}">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" style="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="12">
+        <v>-1</v>
+      </c>
+      <c r="C2" s="17">
+        <v>2.67271619083513E-2</v>
+      </c>
+      <c r="D2" s="17">
+        <v>2.72678689145332E-2</v>
+      </c>
+      <c r="E2" s="17">
+        <v>3.2096028797870102E-2</v>
+      </c>
+      <c r="G2" s="17">
+        <v>-2.2743847892436801</v>
+      </c>
+      <c r="H2" s="17">
+        <v>0</v>
+      </c>
+      <c r="I2" s="17">
+        <v>1.2035689732789301</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="12">
+        <v>0</v>
+      </c>
+      <c r="B3" s="17">
+        <v>1.9010931478256599E-2</v>
+      </c>
+      <c r="C3" s="17">
+        <v>1.23314592183344E-2</v>
+      </c>
+      <c r="D3" s="17">
+        <v>3.24356412684558E-2</v>
+      </c>
+      <c r="E3" s="17">
+        <v>4.0082702640482297E-2</v>
+      </c>
+      <c r="F3" s="17">
+        <v>2.1116786276955</v>
+      </c>
+      <c r="G3" s="17">
+        <v>3.0396191588374699</v>
+      </c>
+      <c r="H3" s="17">
+        <v>0</v>
+      </c>
+      <c r="I3" s="17">
+        <v>1.20461507636536</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="12">
+        <v>1</v>
+      </c>
+      <c r="C4" s="17">
+        <v>2.67271619083672E-2</v>
+      </c>
+      <c r="D4" s="17">
+        <v>2.72678689145479E-2</v>
+      </c>
+      <c r="E4" s="17">
+        <v>3.2096028797896602E-2</v>
+      </c>
+      <c r="G4" s="17">
+        <v>-2.27438478923973</v>
+      </c>
+      <c r="H4" s="17">
+        <v>0</v>
+      </c>
+      <c r="I4" s="17">
+        <v>1.2035689732786901</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FDA1F26-81F4-914D-9042-C84EC2FA5C7C}">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="18">
+        <v>-1</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19">
+        <v>3.0177069026140299E-2</v>
+      </c>
+      <c r="D2" s="19">
+        <v>2.5369338314113199E-2</v>
+      </c>
+      <c r="E2" s="19">
+        <v>3.9722580168397199E-2</v>
+      </c>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19">
+        <v>-2.3298382043552599</v>
+      </c>
+      <c r="H2" s="19">
+        <v>0</v>
+      </c>
+      <c r="I2" s="19">
+        <v>1.16163767666846</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="18">
+        <v>0</v>
+      </c>
+      <c r="B3" s="19">
+        <v>1.9174787614450999E-2</v>
+      </c>
+      <c r="C3" s="19">
+        <v>3.7663549922265997E-2</v>
+      </c>
+      <c r="D3" s="19">
+        <v>2.9016628215863201E-2</v>
+      </c>
+      <c r="E3" s="19">
+        <v>4.8385459601709903E-2</v>
+      </c>
+      <c r="F3" s="19">
+        <v>2.3385191367081202</v>
+      </c>
+      <c r="G3" s="19">
+        <v>-2.1533817544240801</v>
+      </c>
+      <c r="H3" s="19">
+        <v>0</v>
+      </c>
+      <c r="I3" s="19">
+        <v>1.16204278848388</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="18">
+        <v>1</v>
+      </c>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19">
+        <v>3.0177069026091199E-2</v>
+      </c>
+      <c r="D4" s="19">
+        <v>2.5369338314080999E-2</v>
+      </c>
+      <c r="E4" s="19">
+        <v>3.9722580168358397E-2</v>
+      </c>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19">
+        <v>-2.3298382043542101</v>
+      </c>
+      <c r="H4" s="19">
+        <v>0</v>
+      </c>
+      <c r="I4" s="19">
+        <v>1.16163767666037</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AC5FA88-BF56-C34B-9EE3-7E83998CCDD4}">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="18">
+        <v>-1</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19">
+        <v>3.7863243755503302E-3</v>
+      </c>
+      <c r="D2" s="19">
+        <v>1.8211157434347001E-2</v>
+      </c>
+      <c r="E2" s="19">
+        <v>2.4010280697251401E-2</v>
+      </c>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19">
+        <v>2.4509470689294499</v>
+      </c>
+      <c r="H2" s="19">
+        <v>0</v>
+      </c>
+      <c r="I2" s="19">
+        <v>1.2596433010124599</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="18">
+        <v>0</v>
+      </c>
+      <c r="B3" s="19">
+        <v>1.10768427355871E-2</v>
+      </c>
+      <c r="C3" s="19">
+        <v>1.64628443351349E-2</v>
+      </c>
+      <c r="D3" s="19">
+        <v>2.2229781471199399E-2</v>
+      </c>
+      <c r="E3" s="19">
+        <v>3.0305408499985202E-2</v>
+      </c>
+      <c r="F3" s="19">
+        <v>1.80594217139882</v>
+      </c>
+      <c r="G3" s="19">
+        <v>-2.2303538702214998</v>
+      </c>
+      <c r="H3" s="19">
+        <v>0</v>
+      </c>
+      <c r="I3" s="19">
+        <v>1.26585781298393</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="18">
+        <v>1</v>
+      </c>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19">
+        <v>3.78632437579652E-3</v>
+      </c>
+      <c r="D4" s="19">
+        <v>1.82111574341727E-2</v>
+      </c>
+      <c r="E4" s="19">
+        <v>2.40102806971823E-2</v>
+      </c>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19">
+        <v>2.4509470689265398</v>
+      </c>
+      <c r="H4" s="19">
+        <v>0</v>
+      </c>
+      <c r="I4" s="19">
+        <v>1.2596433010049299</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{436344CE-FBA7-FA45-99A0-B52AC1980E06}">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="18">
+        <v>-1</v>
+      </c>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19">
+        <v>2.6730806197423101E-2</v>
+      </c>
+      <c r="D2" s="19">
+        <v>4.05121632609729E-2</v>
+      </c>
+      <c r="E2" s="19">
+        <v>3.2047308922126601E-2</v>
+      </c>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19">
+        <v>-2.2740413240000001</v>
+      </c>
+      <c r="H2" s="19">
+        <v>-1.07E-17</v>
+      </c>
+      <c r="I2" s="19">
+        <v>1.202707344</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="18">
+        <v>0</v>
+      </c>
+      <c r="B3" s="19">
+        <v>2.8253476212569E-2</v>
+      </c>
+      <c r="C3" s="19">
+        <v>1.2300781761591601E-2</v>
+      </c>
+      <c r="D3" s="19">
+        <v>4.8181989165123201E-2</v>
+      </c>
+      <c r="E3" s="19">
+        <v>4.0032656123893E-2</v>
+      </c>
+      <c r="F3" s="19">
+        <v>2.1119789359999999</v>
+      </c>
+      <c r="G3" s="19">
+        <v>3.0409384479999999</v>
+      </c>
+      <c r="H3" s="19">
+        <v>0</v>
+      </c>
+      <c r="I3" s="19">
+        <v>1.203680919</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="18">
+        <v>1</v>
+      </c>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19">
+        <v>2.6730806197585499E-2</v>
+      </c>
+      <c r="D4" s="19">
+        <v>4.0512163261169298E-2</v>
+      </c>
+      <c r="E4" s="19">
+        <v>3.2047308922363502E-2</v>
+      </c>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19">
+        <v>-2.2740413240000001</v>
+      </c>
+      <c r="H4" s="19">
+        <v>0</v>
+      </c>
+      <c r="I4" s="19">
+        <v>1.202707344</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F572B592-A878-A74C-81FF-84D0E863DFE0}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="20"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="12">
+        <v>-1</v>
+      </c>
+      <c r="D2" s="17">
+        <f>-SQRT(15)/10</f>
+        <v>-0.3872983346207417</v>
+      </c>
+      <c r="E2" s="17">
+        <f>SQRT(2)/2</f>
+        <v>0.70710678118654757</v>
+      </c>
+      <c r="F2" s="17">
+        <f>2*SQRT(15)/15</f>
+        <v>0.51639777949432231</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="12">
+        <v>0</v>
+      </c>
+      <c r="B3" s="17">
+        <f>-SQRT(3)/3</f>
+        <v>-0.57735026918962573</v>
+      </c>
+      <c r="C3" s="17">
+        <f>-SQRT(3)/3</f>
+        <v>-0.57735026918962573</v>
+      </c>
+      <c r="D3" s="17">
+        <f>-2*SQRT(15)/15</f>
+        <v>-0.51639777949432231</v>
+      </c>
+      <c r="E3" s="17">
+        <f>SQRT(6)/3</f>
+        <v>0.81649658092772592</v>
+      </c>
+      <c r="F3" s="17">
+        <f>SQRT(10)/5</f>
+        <v>0.63245553203367588</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="12">
+        <v>1</v>
+      </c>
+      <c r="D4" s="17">
+        <f>-SQRT(15)/10</f>
+        <v>-0.3872983346207417</v>
+      </c>
+      <c r="E4" s="17">
+        <f>SQRT(2)/2</f>
+        <v>0.70710678118654757</v>
+      </c>
+      <c r="F4" s="17">
+        <f>2*SQRT(15)/15</f>
+        <v>0.51639777949432231</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>